<commit_message>
validate code has been altered
</commit_message>
<xml_diff>
--- a/com.tp.vTiger/testScriptData/vTiger_testdata.xlsx
+++ b/com.tp.vTiger/testScriptData/vTiger_testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\com.tp.vTiger\testScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\repository\com.tp.vTiger\testScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC4B72A-5580-41B3-A231-BBF42CCF8B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F1667F-6E55-4D0D-B0FC-332CA8996237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{80F69A37-1FD2-4E6F-9537-297052971FE2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t xml:space="preserve">TC_ID </t>
   </si>
@@ -73,12 +73,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Partner</t>
-  </si>
-  <si>
     <t>TC_03</t>
   </si>
   <si>
@@ -91,21 +85,9 @@
     <t>Create Contact</t>
   </si>
   <si>
-    <t>T_P_</t>
-  </si>
-  <si>
-    <t>9874563201</t>
-  </si>
-  <si>
-    <t>Tek_</t>
-  </si>
-  <si>
     <t>Vendorname</t>
   </si>
   <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
     <t>Create Vendor</t>
   </si>
   <si>
@@ -124,9 +106,6 @@
     <t>lead</t>
   </si>
   <si>
-    <t>NoteBook_</t>
-  </si>
-  <si>
     <t>TC_07</t>
   </si>
   <si>
@@ -142,9 +121,6 @@
     <t>LeadSource</t>
   </si>
   <si>
-    <t>Engineering</t>
-  </si>
-  <si>
     <t>Delete Product</t>
   </si>
   <si>
@@ -157,10 +133,37 @@
     <t>Product Name</t>
   </si>
   <si>
-    <t>Pencil_</t>
-  </si>
-  <si>
     <t>Kumar_</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Press</t>
+  </si>
+  <si>
+    <t>TKP_</t>
+  </si>
+  <si>
+    <t>TekP_</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Web Site</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Books_</t>
+  </si>
+  <si>
+    <t>Pen_</t>
+  </si>
+  <si>
+    <t>9760456233</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,13 +611,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -628,21 +631,21 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +658,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,10 +683,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -696,7 +699,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,18 +716,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +740,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,21 +761,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -786,10 +789,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -797,22 +800,22 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -825,7 +828,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -850,10 +853,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -864,10 +867,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -875,13 +878,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>